<commit_message>
update kabupaten bandung barat data
</commit_message>
<xml_diff>
--- a/Dataset/kecamatan_kabupaten_bandung_barat.xlsx
+++ b/Dataset/kecamatan_kabupaten_bandung_barat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Colab Notebooks\Pacmann AI\Statistics\5-Sampling\Project\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD2482D9-F885-480D-9E9B-7B409D8D5C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B684548E-FBE0-4636-A7C2-17EEB66BA55A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="4" xr2:uid="{07BEE02D-3010-4EB1-8920-215C321601A1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{07BEE02D-3010-4EB1-8920-215C321601A1}"/>
   </bookViews>
   <sheets>
     <sheet name="kecamatan_kab_bandung_barat" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="92">
   <si>
     <t>Kecamatan</t>
   </si>
@@ -262,9 +262,6 @@
   </si>
   <si>
     <t>Kepadatan Penduduk (2021)</t>
-  </si>
-  <si>
-    <t>CIlilin</t>
   </si>
   <si>
     <t>Kelompok Umur</t>
@@ -364,9 +361,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
@@ -736,240 +732,240 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>55</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" t="s">
         <v>57</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>59</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" t="s">
         <v>61</v>
       </c>
     </row>
@@ -997,200 +993,200 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>113.12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>160.63999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>120.47</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>77.790000000000006</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>46.99</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>79.959999999999994</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>32.04</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>51.46</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>126.05</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>51.4</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <v>36.01</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>45.15</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>95.56</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>95.56</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>55.11</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <v>112.93</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <v>101.09</v>
       </c>
     </row>
@@ -1215,308 +1211,308 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>60666</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>61507</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>0.15</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>1.59</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>79175</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>80135</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>0.14000000000000001</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>1.42</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>73458</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>74604</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>0.11</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>1.77</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>95470</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>96892</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>0.06</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>1.7</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>132659</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>135732</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>2.5299999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>99991</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>101744</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>0.11</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>1.96</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>107835</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>109877</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <v>2.1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>33820</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>34461</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>0.08</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <v>2.1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>140301</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>142221</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <v>0.04</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="1">
         <v>1.58</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>181359</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>183700</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>0.03</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="1">
         <v>1.5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>177690</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <v>179782</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <v>0.05</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="1">
         <v>1.38</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>113005</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>114372</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1">
         <v>0.08</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="1">
         <v>1.42</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>197640</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>199756</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="1">
         <v>1.28</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>79154</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>80298</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="1">
         <v>0.06</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="1">
         <v>1.65</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>128106</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>129919</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="1">
         <v>0.09</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="1">
         <v>1.62</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>88007</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <v>89226</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="1">
         <v>1.59</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>1788336</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <v>1814226</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="1">
         <v>1.65</v>
       </c>
     </row>
@@ -1529,8 +1525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6142F8CC-24DC-492C-8C21-32E9EC2FB1C6}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1541,308 +1537,308 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>3.39</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>3.39</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>536.29999999999995</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>543.70000000000005</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>4.43</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>4.42</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>492.9</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>498.8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>4.1100000000000003</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>4.1100000000000003</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>609.79999999999995</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>619.29999999999995</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5" s="2">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1">
         <v>5.34</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>5.34</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>1227.3</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>1245.5999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>7.42</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>7.48</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>2823.1</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>2888.5</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>5.59</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>5.61</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>1250.5</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>1272.4000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>6.03</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>6.06</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>3365.6</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <v>3429.4</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>1.89</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>1.9</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>657.2</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <v>669.7</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>7.85</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>7.84</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <v>1113.0999999999999</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="1">
         <v>1128.3</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>10.14</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>10.130000000000001</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>3528.4</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="1">
         <v>3573.9</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>9.94</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <v>9.91</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <v>4934.5</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="1">
         <v>4992.6000000000004</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>6.32</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>6.3</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1">
         <v>2502.9</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="1">
         <v>2533.1999999999998</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>11.05</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>11.01</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <v>2068.1999999999998</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="1">
         <v>2090.4</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>4.43</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>4.43</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="1">
         <v>1436.3</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="1">
         <v>1457</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>7.16</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>7.16</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="1">
         <v>1134.4000000000001</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="1">
         <v>1150.4000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>4.92</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <v>4.92</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="1">
         <v>870.6</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="1">
         <v>882.6</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>100</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <v>100</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="1">
         <v>1369.6</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="1">
         <v>1389.4</v>
       </c>
     </row>
@@ -1855,7 +1851,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09831E24-332E-43B9-ADC5-FB0ABF36B820}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1868,226 +1864,226 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="1">
+        <v>75999</v>
+      </c>
+      <c r="C2" s="1">
+        <v>72689</v>
+      </c>
+      <c r="D2" s="1">
+        <v>148668</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="1">
+        <v>75563</v>
+      </c>
+      <c r="C3" s="1">
+        <v>71631</v>
+      </c>
+      <c r="D3" s="1">
+        <v>147194</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="1">
+        <v>78289</v>
+      </c>
+      <c r="C4" s="1">
+        <v>74008</v>
+      </c>
+      <c r="D4" s="1">
+        <v>152297</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="2">
-        <v>75999</v>
-      </c>
-      <c r="C2" s="2">
-        <v>72689</v>
-      </c>
-      <c r="D2" s="2">
-        <v>148668</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B3" s="2">
-        <v>75563</v>
-      </c>
-      <c r="C3" s="2">
-        <v>71631</v>
-      </c>
-      <c r="D3" s="2">
-        <v>147194</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B4" s="2">
-        <v>78289</v>
-      </c>
-      <c r="C4" s="2">
-        <v>74008</v>
-      </c>
-      <c r="D4" s="2">
-        <v>152297</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="B5" s="1">
+        <v>82345</v>
+      </c>
+      <c r="C5" s="1">
+        <v>76923</v>
+      </c>
+      <c r="D5" s="1">
+        <v>159268</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B5" s="2">
-        <v>82345</v>
-      </c>
-      <c r="C5" s="2">
-        <v>76923</v>
-      </c>
-      <c r="D5" s="2">
-        <v>159268</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="B6" s="1">
+        <v>79406</v>
+      </c>
+      <c r="C6" s="1">
+        <v>73491</v>
+      </c>
+      <c r="D6" s="1">
+        <v>152897</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B6" s="2">
-        <v>79406</v>
-      </c>
-      <c r="C6" s="2">
-        <v>73491</v>
-      </c>
-      <c r="D6" s="2">
-        <v>152897</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="B7" s="1">
+        <v>76409</v>
+      </c>
+      <c r="C7" s="1">
+        <v>73470</v>
+      </c>
+      <c r="D7" s="1">
+        <v>149879</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="2">
-        <v>76409</v>
-      </c>
-      <c r="C7" s="2">
-        <v>73470</v>
-      </c>
-      <c r="D7" s="2">
-        <v>149879</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="B8" s="1">
+        <v>70815</v>
+      </c>
+      <c r="C8" s="1">
+        <v>68736</v>
+      </c>
+      <c r="D8" s="1">
+        <v>139551</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B8" s="2">
-        <v>70815</v>
-      </c>
-      <c r="C8" s="2">
-        <v>68736</v>
-      </c>
-      <c r="D8" s="2">
-        <v>139551</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="B9" s="1">
+        <v>71251</v>
+      </c>
+      <c r="C9" s="1">
+        <v>69427</v>
+      </c>
+      <c r="D9" s="1">
+        <v>140678</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B9" s="2">
-        <v>71251</v>
-      </c>
-      <c r="C9" s="2">
-        <v>69427</v>
-      </c>
-      <c r="D9" s="2">
-        <v>140678</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="B10" s="1">
+        <v>67914</v>
+      </c>
+      <c r="C10" s="1">
+        <v>65803</v>
+      </c>
+      <c r="D10" s="1">
+        <v>133717</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="2">
-        <v>67914</v>
-      </c>
-      <c r="C10" s="2">
-        <v>65803</v>
-      </c>
-      <c r="D10" s="2">
-        <v>133717</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="B11" s="1">
+        <v>61943</v>
+      </c>
+      <c r="C11" s="1">
+        <v>61266</v>
+      </c>
+      <c r="D11" s="1">
+        <v>123209</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B11" s="2">
-        <v>61943</v>
-      </c>
-      <c r="C11" s="2">
-        <v>61266</v>
-      </c>
-      <c r="D11" s="2">
-        <v>123209</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="B12" s="1">
+        <v>52425</v>
+      </c>
+      <c r="C12" s="1">
+        <v>50996</v>
+      </c>
+      <c r="D12" s="1">
+        <v>103421</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B12" s="2">
-        <v>52425</v>
-      </c>
-      <c r="C12" s="2">
-        <v>50996</v>
-      </c>
-      <c r="D12" s="2">
-        <v>103421</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="B13" s="1">
+        <v>44493</v>
+      </c>
+      <c r="C13" s="1">
+        <v>42492</v>
+      </c>
+      <c r="D13" s="1">
+        <v>86985</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B13" s="2">
-        <v>44493</v>
-      </c>
-      <c r="C13" s="2">
-        <v>42492</v>
-      </c>
-      <c r="D13" s="2">
-        <v>86985</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="B14" s="1">
+        <v>25037</v>
+      </c>
+      <c r="C14" s="1">
+        <v>24091</v>
+      </c>
+      <c r="D14" s="1">
+        <v>49128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B14" s="2">
-        <v>25037</v>
-      </c>
-      <c r="C14" s="2">
-        <v>24091</v>
-      </c>
-      <c r="D14" s="2">
-        <v>49128</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="B15" s="1">
+        <v>15392</v>
+      </c>
+      <c r="C15" s="1">
+        <v>15406</v>
+      </c>
+      <c r="D15" s="1">
+        <v>30798</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B15" s="2">
-        <v>15392</v>
-      </c>
-      <c r="C15" s="2">
-        <v>15406</v>
-      </c>
-      <c r="D15" s="2">
-        <v>30798</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>14847</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>15992</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="1">
         <v>30839</v>
       </c>
     </row>

</xml_diff>